<commit_message>
updated the directories and added new dataset for testing
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melicias/Documents/projeto CIIC - inovmineral/newTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581CE6F7-2082-884F-9B33-F8FAA79986FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A2D400-4FCB-214E-892C-1B004BA5AB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19220" xr2:uid="{36346CD8-3FE4-D448-8DD5-31CF691BD5A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="143">
   <si>
     <t>Backdoor</t>
   </si>
@@ -441,6 +441,30 @@
   </si>
   <si>
     <t>0.913852</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>92.28%</t>
+  </si>
+  <si>
+    <t>93.39%</t>
+  </si>
+  <si>
+    <t>92.21%</t>
+  </si>
+  <si>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>0.784786</t>
+  </si>
+  <si>
+    <t>dataset com 250.000 SMOTENC</t>
   </si>
 </sst>
 </file>
@@ -801,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A463B7D-D319-AA4C-87A7-ECB070DEF2AC}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,19 +836,20 @@
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="28.1640625" customWidth="1"/>
-    <col min="4" max="5" width="26" customWidth="1"/>
+    <col min="4" max="5" width="26.1640625" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
     <col min="7" max="8" width="26.5" customWidth="1"/>
-    <col min="9" max="9" width="31.5" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" customWidth="1"/>
-    <col min="14" max="14" width="15.5" customWidth="1"/>
-    <col min="16" max="16" width="24.83203125" customWidth="1"/>
-    <col min="17" max="17" width="25.83203125" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="28.5" customWidth="1"/>
+    <col min="10" max="10" width="31.5" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.5" customWidth="1"/>
+    <col min="17" max="17" width="24.83203125" customWidth="1"/>
+    <col min="18" max="18" width="25.83203125" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
@@ -834,23 +859,24 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>16</v>
       </c>
@@ -870,37 +896,40 @@
         <v>110</v>
       </c>
       <c r="I2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" t="s">
         <v>41</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>55</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>60</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>70</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>80</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>81</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>82</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>88</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>89</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>29</v>
       </c>
@@ -949,8 +978,11 @@
       <c r="R3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="S3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -973,34 +1005,37 @@
         <v>32</v>
       </c>
       <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>32</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>75</v>
       </c>
-      <c r="N4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="O4" t="s">
         <v>32</v>
       </c>
       <c r="Q4" t="s">
         <v>32</v>
       </c>
       <c r="R4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1023,34 +1058,37 @@
         <v>33</v>
       </c>
       <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
         <v>43</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>61</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>18</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>19</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>25</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>49</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -1085,12 +1123,12 @@
         <v>23</v>
       </c>
       <c r="M6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" t="s">
         <v>76</v>
       </c>
-      <c r="N6" t="s">
-        <v>23</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="O6" t="s">
         <v>23</v>
       </c>
       <c r="Q6" t="s">
@@ -1099,8 +1137,11 @@
       <c r="R6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="S6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1135,22 +1176,25 @@
         <v>23</v>
       </c>
       <c r="M7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" t="s">
         <v>25</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>45</v>
       </c>
-      <c r="P7" t="s">
-        <v>23</v>
-      </c>
       <c r="Q7" t="s">
         <v>23</v>
       </c>
       <c r="R7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="S7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1234,7 @@
       <c r="N8" t="s">
         <v>23</v>
       </c>
-      <c r="P8" t="s">
+      <c r="O8" t="s">
         <v>23</v>
       </c>
       <c r="Q8" t="s">
@@ -1199,8 +1243,11 @@
       <c r="R8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="S8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1223,34 +1270,37 @@
         <v>124</v>
       </c>
       <c r="I9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" t="s">
         <v>44</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>47</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>62</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>61</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>77</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>36</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>35</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1323,7 @@
         <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="J10" t="s">
         <v>23</v>
@@ -1285,22 +1335,25 @@
         <v>23</v>
       </c>
       <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
         <v>56</v>
       </c>
-      <c r="N10" t="s">
-        <v>23</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="O10" t="s">
         <v>23</v>
       </c>
       <c r="Q10" t="s">
         <v>23</v>
       </c>
       <c r="R10" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -1340,7 +1393,7 @@
       <c r="N11" t="s">
         <v>23</v>
       </c>
-      <c r="P11" t="s">
+      <c r="O11" t="s">
         <v>23</v>
       </c>
       <c r="Q11" t="s">
@@ -1349,8 +1402,11 @@
       <c r="R11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -1373,34 +1429,37 @@
         <v>85</v>
       </c>
       <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
         <v>34</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>19</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>39</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>21</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>62</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>83</v>
-      </c>
-      <c r="P12" t="s">
-        <v>75</v>
       </c>
       <c r="Q12" t="s">
         <v>75</v>
       </c>
       <c r="R12" t="s">
+        <v>75</v>
+      </c>
+      <c r="S12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -1423,34 +1482,37 @@
         <v>17</v>
       </c>
       <c r="I13" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" t="s">
         <v>45</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>56</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>63</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>56</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>77</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>84</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>56</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>32</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1476,31 +1538,34 @@
         <v>46</v>
       </c>
       <c r="J14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" t="s">
         <v>20</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>45</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>20</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>66</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>49</v>
-      </c>
-      <c r="P14" t="s">
-        <v>20</v>
       </c>
       <c r="Q14" t="s">
         <v>20</v>
       </c>
       <c r="R14" t="s">
+        <v>20</v>
+      </c>
+      <c r="S14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -1523,25 +1588,25 @@
         <v>125</v>
       </c>
       <c r="I15" t="s">
+        <v>99</v>
+      </c>
+      <c r="J15" t="s">
         <v>47</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>25</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>64</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>19</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>40</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>39</v>
-      </c>
-      <c r="P15" t="s">
-        <v>37</v>
       </c>
       <c r="Q15" t="s">
         <v>37</v>
@@ -1549,8 +1614,11 @@
       <c r="R15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="S15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -1573,34 +1641,37 @@
         <v>38</v>
       </c>
       <c r="I16" t="s">
+        <v>136</v>
+      </c>
+      <c r="J16" t="s">
         <v>48</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>22</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>65</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>57</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>78</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>85</v>
-      </c>
-      <c r="P16" t="s">
-        <v>75</v>
       </c>
       <c r="Q16" t="s">
         <v>75</v>
       </c>
       <c r="R16" t="s">
+        <v>75</v>
+      </c>
+      <c r="S16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -1626,31 +1697,34 @@
         <v>49</v>
       </c>
       <c r="J17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" t="s">
         <v>32</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>20</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>17</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>19</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>45</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>56</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>32</v>
       </c>
       <c r="R17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -1673,34 +1747,37 @@
         <v>40</v>
       </c>
       <c r="I18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" t="s">
         <v>50</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>57</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>66</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>57</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>79</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>86</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>46</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>75</v>
       </c>
       <c r="R18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>26</v>
       </c>
@@ -1723,28 +1800,31 @@
         <v>126</v>
       </c>
       <c r="I20" t="s">
+        <v>137</v>
+      </c>
+      <c r="J20" t="s">
         <v>51</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>58</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>67</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>71</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>92</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>91</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>27</v>
       </c>
@@ -1767,19 +1847,22 @@
         <v>127</v>
       </c>
       <c r="I21" t="s">
+        <v>138</v>
+      </c>
+      <c r="J21" t="s">
         <v>52</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>58</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>68</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>28</v>
       </c>
@@ -1802,19 +1885,22 @@
         <v>126</v>
       </c>
       <c r="I22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J22" t="s">
         <v>51</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>58</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>67</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>30</v>
       </c>
@@ -1837,19 +1923,22 @@
         <v>128</v>
       </c>
       <c r="I23" t="s">
+        <v>139</v>
+      </c>
+      <c r="J23" t="s">
         <v>53</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>59</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>69</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>97</v>
       </c>
@@ -1874,8 +1963,11 @@
       <c r="H24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
         <v>28</v>
@@ -1898,8 +1990,11 @@
       <c r="H25" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
         <v>30</v>
@@ -1922,8 +2017,11 @@
       <c r="H26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>98</v>
       </c>
@@ -1948,8 +2046,11 @@
       <c r="H27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
         <v>28</v>
@@ -1972,8 +2073,11 @@
       <c r="H28" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
         <v>30</v>
@@ -1996,8 +2100,11 @@
       <c r="H29" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>101</v>
       </c>
@@ -2018,15 +2125,18 @@
       </c>
       <c r="H30" t="s">
         <v>129</v>
+      </c>
+      <c r="I30" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A27:A29"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A24:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SMOTENC testes with 2022 dataset IVO
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melicias/Documents/projeto CIIC - inovmineral/newTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99863EC9-6998-9F4C-B7FC-4D8C9EBFB7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE75814D-1D37-B343-B6AF-3DE75A40684C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19220" xr2:uid="{36346CD8-3FE4-D448-8DD5-31CF691BD5A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="195">
   <si>
     <t>Backdoor</t>
   </si>
@@ -600,6 +600,27 @@
   </si>
   <si>
     <t>0.791810</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.43</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>0.683398</t>
+  </si>
+  <si>
+    <t>0.39</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.801988</t>
   </si>
 </sst>
 </file>
@@ -963,7 +984,7 @@
   <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2330,6 +2351,12 @@
       <c r="G35" t="s">
         <v>35</v>
       </c>
+      <c r="H35" t="s">
+        <v>188</v>
+      </c>
+      <c r="I35" t="s">
+        <v>192</v>
+      </c>
       <c r="J35" t="s">
         <v>179</v>
       </c>
@@ -2353,6 +2380,12 @@
       <c r="G36" t="s">
         <v>77</v>
       </c>
+      <c r="H36" t="s">
+        <v>77</v>
+      </c>
+      <c r="I36" t="s">
+        <v>77</v>
+      </c>
       <c r="J36" t="s">
         <v>77</v>
       </c>
@@ -2376,6 +2409,12 @@
       <c r="G37" t="s">
         <v>38</v>
       </c>
+      <c r="H37" t="s">
+        <v>189</v>
+      </c>
+      <c r="I37" t="s">
+        <v>36</v>
+      </c>
       <c r="J37" t="s">
         <v>180</v>
       </c>
@@ -2399,6 +2438,12 @@
       <c r="G38" t="s">
         <v>76</v>
       </c>
+      <c r="H38" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" t="s">
+        <v>76</v>
+      </c>
       <c r="J38" t="s">
         <v>56</v>
       </c>
@@ -2422,6 +2467,12 @@
       <c r="G39" t="s">
         <v>23</v>
       </c>
+      <c r="H39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" t="s">
+        <v>23</v>
+      </c>
       <c r="J39" t="s">
         <v>23</v>
       </c>
@@ -2445,6 +2496,12 @@
       <c r="G40" t="s">
         <v>76</v>
       </c>
+      <c r="H40" t="s">
+        <v>56</v>
+      </c>
+      <c r="I40" t="s">
+        <v>56</v>
+      </c>
       <c r="J40" t="s">
         <v>76</v>
       </c>
@@ -2468,6 +2525,12 @@
       <c r="G41" t="s">
         <v>162</v>
       </c>
+      <c r="H41" t="s">
+        <v>166</v>
+      </c>
+      <c r="I41" t="s">
+        <v>193</v>
+      </c>
       <c r="J41" t="s">
         <v>47</v>
       </c>
@@ -2491,6 +2554,12 @@
       <c r="G42" t="s">
         <v>24</v>
       </c>
+      <c r="H42" t="s">
+        <v>93</v>
+      </c>
+      <c r="I42" t="s">
+        <v>24</v>
+      </c>
       <c r="J42" t="s">
         <v>84</v>
       </c>
@@ -2514,6 +2583,12 @@
       <c r="G43" t="s">
         <v>18</v>
       </c>
+      <c r="H43" t="s">
+        <v>190</v>
+      </c>
+      <c r="I43" t="s">
+        <v>25</v>
+      </c>
       <c r="J43" t="s">
         <v>20</v>
       </c>
@@ -2537,6 +2612,12 @@
       <c r="G44" t="s">
         <v>23</v>
       </c>
+      <c r="H44" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" t="s">
+        <v>23</v>
+      </c>
       <c r="J44" t="s">
         <v>23</v>
       </c>
@@ -2560,6 +2641,12 @@
       <c r="G46" t="s">
         <v>158</v>
       </c>
+      <c r="H46" t="s">
+        <v>181</v>
+      </c>
+      <c r="I46" t="s">
+        <v>181</v>
+      </c>
       <c r="J46" t="s">
         <v>181</v>
       </c>
@@ -2583,6 +2670,12 @@
       <c r="G47" t="s">
         <v>185</v>
       </c>
+      <c r="H47" t="s">
+        <v>181</v>
+      </c>
+      <c r="I47" t="s">
+        <v>181</v>
+      </c>
       <c r="J47" t="s">
         <v>181</v>
       </c>
@@ -2606,6 +2699,12 @@
       <c r="G48" t="s">
         <v>158</v>
       </c>
+      <c r="H48" t="s">
+        <v>181</v>
+      </c>
+      <c r="I48" t="s">
+        <v>181</v>
+      </c>
       <c r="J48" t="s">
         <v>181</v>
       </c>
@@ -2629,6 +2728,12 @@
       <c r="G49" t="s">
         <v>186</v>
       </c>
+      <c r="H49" t="s">
+        <v>181</v>
+      </c>
+      <c r="I49" t="s">
+        <v>181</v>
+      </c>
       <c r="J49" t="s">
         <v>181</v>
       </c>
@@ -2654,6 +2759,12 @@
       </c>
       <c r="G50" t="s">
         <v>61</v>
+      </c>
+      <c r="H50" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" t="s">
+        <v>24</v>
       </c>
       <c r="J50" t="s">
         <v>166</v>
@@ -2679,6 +2790,12 @@
       <c r="G51" t="s">
         <v>57</v>
       </c>
+      <c r="H51" t="s">
+        <v>93</v>
+      </c>
+      <c r="I51" t="s">
+        <v>21</v>
+      </c>
       <c r="J51" t="s">
         <v>61</v>
       </c>
@@ -2703,6 +2820,12 @@
       <c r="G52" t="s">
         <v>48</v>
       </c>
+      <c r="H52" t="s">
+        <v>136</v>
+      </c>
+      <c r="I52" t="s">
+        <v>93</v>
+      </c>
       <c r="J52" t="s">
         <v>61</v>
       </c>
@@ -2728,6 +2851,12 @@
       </c>
       <c r="G53" t="s">
         <v>56</v>
+      </c>
+      <c r="H53" t="s">
+        <v>32</v>
+      </c>
+      <c r="I53" t="s">
+        <v>32</v>
       </c>
       <c r="J53" t="s">
         <v>32</v>
@@ -2753,6 +2882,12 @@
       <c r="G54" t="s">
         <v>32</v>
       </c>
+      <c r="H54" t="s">
+        <v>32</v>
+      </c>
+      <c r="I54" t="s">
+        <v>42</v>
+      </c>
       <c r="J54" t="s">
         <v>32</v>
       </c>
@@ -2777,6 +2912,12 @@
       <c r="G55" t="s">
         <v>32</v>
       </c>
+      <c r="H55" t="s">
+        <v>32</v>
+      </c>
+      <c r="I55" t="s">
+        <v>42</v>
+      </c>
       <c r="J55" t="s">
         <v>32</v>
       </c>
@@ -2799,6 +2940,12 @@
       </c>
       <c r="G56" t="s">
         <v>187</v>
+      </c>
+      <c r="H56" t="s">
+        <v>191</v>
+      </c>
+      <c r="I56" t="s">
+        <v>194</v>
       </c>
       <c r="J56" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
changes to test in VM
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melicias/Documents/projeto CIIC - inovmineral/newTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E81A3F-5D73-CC4F-BE91-B4B0B02497E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FC8836-3876-9B44-9596-3EA0987C6604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19220" xr2:uid="{36346CD8-3FE4-D448-8DD5-31CF691BD5A8}"/>
   </bookViews>
@@ -1037,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A463B7D-D319-AA4C-87A7-ECB070DEF2AC}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="86" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32:M32"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1046,16 +1046,16 @@
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="28.1640625" customWidth="1"/>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="4" max="4" width="44.83203125" customWidth="1"/>
+    <col min="5" max="5" width="49.5" customWidth="1"/>
+    <col min="6" max="6" width="70.6640625" customWidth="1"/>
     <col min="7" max="7" width="26.5" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" customWidth="1"/>
     <col min="9" max="9" width="28.5" customWidth="1"/>
     <col min="10" max="10" width="31.5" customWidth="1"/>
     <col min="11" max="11" width="27.1640625" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="34" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" customWidth="1"/>
     <col min="14" max="14" width="13.1640625" customWidth="1"/>
     <col min="15" max="15" width="16.83203125" customWidth="1"/>
     <col min="16" max="16" width="17.6640625" customWidth="1"/>

</xml_diff>